<commit_message>
Added API TDS Customer Creation and Get Customer
</commit_message>
<xml_diff>
--- a/SoftwareRequirment.xlsx
+++ b/SoftwareRequirment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AnuragStudy\jwt-spring\TaxConsultencyOfficeManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anjani\TaxConsultionOfficeManagement\TaxConsultingOfficeManagmement\TaxConsultencyOfficeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872B3FD9-5D91-4BBC-A0BB-AA20145E574C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09A0E0-5EB9-4C5E-9D98-BFDBFACC764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="12" r:id="rId1"/>
@@ -849,12 +849,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
@@ -862,7 +862,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -870,17 +870,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -898,13 +898,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
@@ -912,33 +912,33 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -946,12 +946,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -959,27 +959,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1000,62 +1000,62 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1073,22 +1073,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1106,52 +1106,52 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" customWidth="1"/>
+    <col min="1" max="1" width="44.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -1169,17 +1169,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="69.77734375" customWidth="1"/>
+    <col min="1" max="1" width="69.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1197,17 +1197,17 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="35.109375" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" customWidth="1"/>
-    <col min="6" max="6" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="35.08984375" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -1227,17 +1227,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>86</v>
       </c>
@@ -1255,18 +1255,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.08984375" customWidth="1"/>
+    <col min="3" max="3" width="44.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1344,18 +1344,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B407ACD3-4B37-492A-8FA0-C86C5BA19DD5}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="148.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="3" max="3" width="148.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>93</v>
       </c>
@@ -1363,19 +1363,19 @@
       <c r="C1" s="8"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>94</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>99</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>105</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H14" s="1"/>
     </row>
   </sheetData>
@@ -1464,7 +1464,7 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1478,12 +1478,12 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
@@ -1491,49 +1491,49 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1554,34 +1554,34 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1602,12 +1602,12 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -1615,54 +1615,54 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1683,13 +1683,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -1697,34 +1697,34 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1732,22 +1732,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1768,12 +1768,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>49</v>
       </c>
@@ -1781,28 +1781,28 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
updated Search based on Request Param
</commit_message>
<xml_diff>
--- a/SoftwareRequirment.xlsx
+++ b/SoftwareRequirment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anjani\TaxConsultionOfficeManagement\TaxConsultingOfficeManagmement\TaxConsultencyOfficeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB09A0E0-5EB9-4C5E-9D98-BFDBFACC764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300ECD7F-26DF-4BC7-8F94-FAA33855A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="12" r:id="rId1"/>
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B407ACD3-4B37-492A-8FA0-C86C5BA19DD5}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1598,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B9D1D6-7050-4F34-BBEF-C07DD4000C89}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Deactivate customer and restore TDS Customer
</commit_message>
<xml_diff>
--- a/SoftwareRequirment.xlsx
+++ b/SoftwareRequirment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anjani\TaxConsultionOfficeManagement\TaxConsultingOfficeManagmement\TaxConsultencyOfficeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300ECD7F-26DF-4BC7-8F94-FAA33855A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55780BCF-66E8-4E9B-986B-55E6B5D615B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="6" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{CD00193F-9A11-4B8F-B22A-766C7E14F037}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -404,6 +404,15 @@
 /tds-customers/{tds-customer-id}
 /tds-customers/{tds-customer-id}
 /tds-customers?name=""&amp;year=""&amp;month=""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restore Deactivated Entity </t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>/restore/tds-customers/{tds-customer-id}</t>
   </si>
 </sst>
 </file>
@@ -500,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,6 +536,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1344,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B407ACD3-4B37-492A-8FA0-C86C5BA19DD5}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1443,6 +1458,17 @@
       </c>
       <c r="D8" s="6" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1598,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47B9D1D6-7050-4F34-BBEF-C07DD4000C89}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>